<commit_message>
8.15 Sprint 1 cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\eclipse-workspace\LYNX_Automation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B600805C-B19E-40FD-BC36-3DA09564C884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559A316-ACCF-4967-AF98-347AE7C6E1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>RunTest</t>
   </si>
@@ -118,6 +118,42 @@
   </si>
   <si>
     <t>Aim is to verify whether a story is published correctly</t>
+  </si>
+  <si>
+    <t>HeadLineSettings22797</t>
+  </si>
+  <si>
+    <t>SetHeadlineTextColor</t>
+  </si>
+  <si>
+    <t>FW_UI_0006</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Aim of the script is to verify that user is able to set text color for the headline</t>
+  </si>
+  <si>
+    <t>Aim of the script is to verify that user is able to set background color for the headline</t>
+  </si>
+  <si>
+    <t>SetHeadlineBGColor</t>
+  </si>
+  <si>
+    <t>FW_UI_0007</t>
+  </si>
+  <si>
+    <t>SetHeadlineBold</t>
+  </si>
+  <si>
+    <t>FW_UI_0008</t>
+  </si>
+  <si>
+    <t>EditExistingHeadlineHighlights</t>
+  </si>
+  <si>
+    <t>FW_UI_0009</t>
   </si>
 </sst>
 </file>
@@ -545,10 +581,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -583,7 +619,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -601,7 +637,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -621,7 +657,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -641,7 +677,7 @@
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -659,7 +695,7 @@
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -677,7 +713,7 @@
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -691,6 +727,78 @@
       </c>
       <c r="F7" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8.15 Sprint1 TEst Cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559A316-ACCF-4967-AF98-347AE7C6E1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53660128-8781-43F8-AA3C-152C113BFB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>RunTest</t>
   </si>
@@ -154,6 +154,57 @@
   </si>
   <si>
     <t>FW_UI_0009</t>
+  </si>
+  <si>
+    <t>FW_UI_0010</t>
+  </si>
+  <si>
+    <t>Reopen</t>
+  </si>
+  <si>
+    <t>Relaunch</t>
+  </si>
+  <si>
+    <t>FW_UI_0011</t>
+  </si>
+  <si>
+    <t>FW_UI_0012</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view headline highlight settings done under alarms list on reopening preferences</t>
+  </si>
+  <si>
+    <t>To verify that headline highlight settings for new and existing alarms are retained on relaunching LE</t>
+  </si>
+  <si>
+    <t>To verify that user is able to set headline without bold option</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>HeadlineOptionReopenRelaunch</t>
+  </si>
+  <si>
+    <t>To verify that user is able to set headline in bold</t>
+  </si>
+  <si>
+    <t>To verify that user is able to set color,font options and preview headline for an existing headline alarm based on the selections made</t>
+  </si>
+  <si>
+    <t>Feeds233961</t>
+  </si>
+  <si>
+    <t>FW_UI_0013</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the the selected feeds under Feeds dropdown in UI</t>
+  </si>
+  <si>
+    <t>VerifyFeedsDropdown</t>
   </si>
 </sst>
 </file>
@@ -581,10 +632,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -775,17 +826,19 @@
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>39</v>
@@ -798,8 +851,158 @@
         <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
8.16 Sprint 2 cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53660128-8781-43F8-AA3C-152C113BFB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E26D31-57ED-4840-9E41-0A7AD1BCE200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>RunTest</t>
   </si>
@@ -205,6 +205,75 @@
   </si>
   <si>
     <t>VerifyFeedsDropdown</t>
+  </si>
+  <si>
+    <t>VerifyFeedinHeadline</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the releases in FW UI based on selected feeds</t>
+  </si>
+  <si>
+    <t>FW_UI_0014</t>
+  </si>
+  <si>
+    <t>Australia,sydney.newsroom,Denmark,copenhagen.newsroom</t>
+  </si>
+  <si>
+    <t>To verify that  user can remove selected feeds Webui preferences</t>
+  </si>
+  <si>
+    <t>FW_UI_0015</t>
+  </si>
+  <si>
+    <t>VerifyFeedRemoval</t>
+  </si>
+  <si>
+    <t>Australia,sydney.newsroom</t>
+  </si>
+  <si>
+    <t>VerifyFeedDeselection</t>
+  </si>
+  <si>
+    <t>To verify that user is able to  deselect feeds  from Feeds dropdown</t>
+  </si>
+  <si>
+    <t>FW_UI_0016</t>
+  </si>
+  <si>
+    <t>To verify that user is able to select feeds  from Feeds dropdown</t>
+  </si>
+  <si>
+    <t>FW_UI_0017</t>
+  </si>
+  <si>
+    <t>FW_UI_0018</t>
+  </si>
+  <si>
+    <t>FW_UI_0019</t>
+  </si>
+  <si>
+    <t>FW_UI_0020</t>
+  </si>
+  <si>
+    <t>FW_UI_0021</t>
+  </si>
+  <si>
+    <t>VerifyFeedReselection</t>
+  </si>
+  <si>
+    <t>VerifyFeedRelaunch</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the releases in FW UI based on selected feeds in relaunched LE</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the releases in FW UI based on selected feeds in torn out tab</t>
+  </si>
+  <si>
+    <t>Australia,sydney.newsroom,Denmark,copenhagen.newsroom,normal</t>
+  </si>
+  <si>
+    <t>Australia,sydney.newsroom,Denmark,copenhagen.newsroom,torn</t>
   </si>
 </sst>
 </file>
@@ -632,10 +701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -748,7 +817,7 @@
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -766,7 +835,7 @@
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -784,7 +853,7 @@
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -858,7 +927,7 @@
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -878,7 +947,7 @@
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -895,114 +964,184 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="B21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updated with more Regression cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/FW_UI_0000.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9535ED6F-F576-4B22-9560-6D4207FF10BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA82D79-67C0-4EBC-9D26-C53F80F7A4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="111">
   <si>
     <t>RunTest</t>
   </si>
@@ -330,19 +330,43 @@
     <t>VerifyAutomationDeselection</t>
   </si>
   <si>
-    <t>FW_UI_0025</t>
-  </si>
-  <si>
     <t>To verify that user is able to  deselect automations  from automations dropdown</t>
   </si>
   <si>
     <t>VerifyAutomationReselection</t>
   </si>
   <si>
-    <t>FE_UI_0026</t>
-  </si>
-  <si>
     <t>To verify that user is able to select automations  from automations dropdown</t>
+  </si>
+  <si>
+    <t>VerifyAutomationRelaunchReopen</t>
+  </si>
+  <si>
+    <t>EarthquakeDailyHandbrake,AustraliaDailyStockHeadlines,Relaunch</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the releases in FW UI based on selected automations in relaunched LE</t>
+  </si>
+  <si>
+    <t>To verify that user is able to view the releases in FW UI based on selected automations in newly opened FW tab</t>
+  </si>
+  <si>
+    <t>EarthquakeDailyHandbrake,AustraliaDailyStockHeadlines,Reopen</t>
+  </si>
+  <si>
+    <t>Aim of the script is to verify that as  a Technical Director, I want to know the usefulness of Story Categorizer component in Fastwire</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>MetaData</t>
+  </si>
+  <si>
+    <t>VerfiyAlertEditor</t>
+  </si>
+  <si>
+    <t>FW_UI_0000</t>
   </si>
 </sst>
 </file>
@@ -511,42 +535,27 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -576,12 +585,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -590,9 +593,7 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -622,6 +623,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -639,6 +655,59 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -679,79 +748,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -760,25 +756,53 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -795,14 +819,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A2:F28" headerRowCount="0" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A2:F31" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="Column1" headerRowDxfId="8" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="Column2" headerRowDxfId="9" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{7C8347B6-FF57-42E1-A6C2-EC27070A40D0}" name="Column3" headerRowDxfId="10" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{EE0534CE-1AD7-4FF9-85D0-3AE501688863}" name="Column4" headerRowDxfId="11" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D9E527CD-0865-44E9-A462-CB70BB730775}" name="Column5" headerRowDxfId="12" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{8264D975-498F-4ED6-8B84-152D38F182B3}" name="Column6" headerRowDxfId="13" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="Column1" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{7C8347B6-FF57-42E1-A6C2-EC27070A40D0}" name="Column3" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{EE0534CE-1AD7-4FF9-85D0-3AE501688863}" name="Column4" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D9E527CD-0865-44E9-A462-CB70BB730775}" name="Column5" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8264D975-498F-4ED6-8B84-152D38F182B3}" name="Column6" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1130,19 +1154,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="28.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1171,7 +1196,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
@@ -1189,7 +1214,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -1209,7 +1234,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
@@ -1229,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>20</v>
@@ -1247,7 +1272,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>16</v>
@@ -1265,7 +1290,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
@@ -1283,7 +1308,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>29</v>
@@ -1301,7 +1326,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>34</v>
@@ -1319,7 +1344,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>36</v>
@@ -1339,7 +1364,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>38</v>
@@ -1357,7 +1382,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>50</v>
@@ -1377,7 +1402,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>50</v>
@@ -1397,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>36</v>
@@ -1417,7 +1442,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>56</v>
@@ -1437,7 +1462,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>57</v>
@@ -1457,7 +1482,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>62</v>
@@ -1477,7 +1502,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>64</v>
@@ -1497,7 +1522,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>72</v>
@@ -1517,7 +1542,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>76</v>
@@ -1537,7 +1562,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>57</v>
@@ -1557,7 +1582,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>76</v>
@@ -1577,7 +1602,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>86</v>
@@ -1597,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>87</v>
@@ -1617,7 +1642,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>87</v>
@@ -1633,11 +1658,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>95</v>
+      <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>96</v>
@@ -1653,43 +1678,103 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>98</v>
+      <c r="A27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>83</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>102</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>